<commit_message>
fix: correccion formato GenContacto
</commit_message>
<xml_diff>
--- a/src/assets/ejemplos/modelo/GenContacto.xlsx
+++ b/src/assets/ejemplos/modelo/GenContacto.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">NUMERO_IDENTIFICACION</t>
   </si>
@@ -94,12 +94,6 @@
     <t xml:space="preserve">soportetecnico@santaelena.com.co</t>
   </si>
   <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI</t>
-  </si>
-  <si>
     <t xml:space="preserve">EMPRESA LTDA</t>
   </si>
   <si>
@@ -110,6 +104,9 @@
   </si>
   <si>
     <t xml:space="preserve">empresa@ltda.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARIA VERONICA GUZMAN CHAVARRIA</t>
   </si>
   <si>
     <t xml:space="preserve">MARIA</t>
@@ -141,7 +138,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +176,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -222,33 +225,37 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -441,8 +448,8 @@
   </sheetPr>
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q14" activeCellId="0" sqref="Q14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -555,14 +562,14 @@
         <v>23</v>
       </c>
       <c r="O2" s="6"/>
-      <c r="P2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>24</v>
+      <c r="P2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" s="6" t="n">
+        <v>0</v>
       </c>
       <c r="S2" s="5" t="n">
         <v>1</v>
@@ -579,13 +586,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="5" t="n">
@@ -598,17 +605,17 @@
         <v>3015678954</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O3" s="6"/>
-      <c r="P3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>24</v>
+      <c r="P3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="6" t="n">
+        <v>0</v>
       </c>
       <c r="S3" s="5" t="n">
         <v>4</v>
@@ -624,23 +631,26 @@
       <c r="B4" s="5" t="n">
         <v>3</v>
       </c>
+      <c r="C4" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="D4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="K4" s="5" t="n">
         <v>1</v>
@@ -652,17 +662,17 @@
         <v>3011234567</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O4" s="6"/>
-      <c r="P4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>25</v>
+      <c r="P4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="6" t="n">
+        <v>1</v>
       </c>
       <c r="S4" s="5" t="n">
         <v>1</v>

</xml_diff>